<commit_message>
[modify] 更新Unity IAP, 按照更新修正支付失败为 DuplicateTransaction 情况的逻辑
</commit_message>
<xml_diff>
--- a/Assets/Plugins/FantaBlade/Res/localize.xlsx
+++ b/Assets/Plugins/FantaBlade/Res/localize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wusongtao\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFCC64C-66DC-460E-80DA-F63421C7FE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E4AA39-FF5B-4FB7-8472-65876A77405E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{68D96789-0ED1-4C4F-B460-67FE1F76A131}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{68D96789-0ED1-4C4F-B460-67FE1F76A131}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="339">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -274,10 +274,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>please_intpu_validate_code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>请输入验证码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -337,9 +333,6 @@
     <t>Please Input Username/Email</t>
   </si>
   <si>
-    <t>Get Verify Code</t>
-  </si>
-  <si>
     <t>Account Login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,13 +345,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Reset Password?</t>
-  </si>
-  <si>
-    <t>Register Account?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Forget Password?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -367,10 +353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Please Intpu Validate Code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Please Confirm Password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -794,9 +776,6 @@
     <t>Syrian Arab Republic</t>
   </si>
   <si>
-    <t>Taiwan</t>
-  </si>
-  <si>
     <t>Tajikistan</t>
   </si>
   <si>
@@ -1229,27 +1208,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>確定退出遊戲嘛？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>確定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>再玩一會兒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Currently for the Tourist account，switching accounts may result in account loss，still have to switch?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorry，the device is temporarily unable to use the quick login feature，please log in after register.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taiwan， Province of China</t>
+  </si>
+  <si>
+    <t>Send</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发 送</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register Account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset Password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Are you sure to quit the game?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>確定退出遊戲嘛？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>確定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>再玩一會兒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Currently for the Tourist account，switching accounts may result in account loss，still have to switch?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sorry，the device is temporarily unable to use the quick login feature，please log in after register.</t>
+    <t>發 送</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please Input Validate Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>please_input_validate_code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1678,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD03A67-A19B-4F89-B488-C4E4A011549E}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1767,7 +1781,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1775,7 +1789,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1783,7 +1797,7 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1791,7 +1805,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1799,7 +1813,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1807,7 +1821,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1815,7 +1829,7 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1823,12 +1837,12 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
         <v>52</v>
@@ -1839,7 +1853,7 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1847,7 +1861,7 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1855,7 +1869,7 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1863,467 +1877,472 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>338</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>206</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>326</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2335,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39947906-DDE0-4C2E-B307-71C44DA6F3AD}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2485,7 +2504,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
@@ -2520,695 +2539,703 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>338</v>
+      </c>
+      <c r="B23" t="s">
         <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
         <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
         <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B33" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B54" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B64" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B65" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B72" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B74" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B80" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B81" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B83" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B84" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B85" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B87" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B88" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B89" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B90" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B93" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>206</v>
+        <v>329</v>
       </c>
       <c r="B94" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B96" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B97" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B98" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B99" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B100" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B101" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B102" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B103" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B104" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B105" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B107" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B108" t="s">
-        <v>327</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>330</v>
+      </c>
+      <c r="B109" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3220,10 +3247,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6BA963-2B65-4518-8D4F-8014EC1EC200}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3317,7 +3344,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3325,7 +3352,7 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3333,7 +3360,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3341,7 +3368,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3349,7 +3376,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3357,7 +3384,7 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3365,15 +3392,15 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3381,7 +3408,7 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3389,7 +3416,7 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3397,7 +3424,7 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3405,695 +3432,703 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>338</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
         <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B33" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B49" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B52" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B53" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B54" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B55" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B58" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B60" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B62" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B64" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B65" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B66" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B68" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B70" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B71" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B72" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B74" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B77" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B80" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B81" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B83" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B84" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B85" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B86" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B87" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B88" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B89" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B90" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B93" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>206</v>
+        <v>329</v>
       </c>
       <c r="B94" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B95" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B96" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B97" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B98" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B99" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B100" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B101" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B102" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B103" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B104" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B105" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B106" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B107" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>320</v>
+      </c>
+      <c r="B108" t="s">
         <v>326</v>
       </c>
-      <c r="B108" t="s">
-        <v>333</v>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>330</v>
+      </c>
+      <c r="B109" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>